<commit_message>
Test cases successfully added. -Cooper
</commit_message>
<xml_diff>
--- a/testcases.xlsx
+++ b/testcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nmare\PycharmProjects\cs151-pa0-CooperNaz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB18B4C-4A3C-4068-8042-48D142FFBE67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C13D31-4BB0-49DF-9B68-F692A020D995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3828" yWindow="3120" windowWidth="17280" windowHeight="10008" xr2:uid="{3FADB8AC-B405-4FE2-9A10-87DD62C18585}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{3FADB8AC-B405-4FE2-9A10-87DD62C18585}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,15 +36,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>IN: Radius (cm)</t>
+  </si>
+  <si>
+    <t>IN: Height (cm)</t>
   </si>
   <si>
     <t>OUT: Volume (ML)</t>
   </si>
   <si>
     <t>OUT: Cups</t>
+  </si>
+  <si>
+    <t>The actual code rounds to the second decimal point. This does not account for that.</t>
   </si>
 </sst>
 </file>
@@ -110,7 +116,32 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -121,6 +152,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{28AF149D-A8D8-4595-ADEB-1444FBDB0EC6}" name="Table1" displayName="Table1" ref="A1:D7" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:D7" xr:uid="{28AF149D-A8D8-4595-ADEB-1444FBDB0EC6}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{0294D113-D76F-46CC-96DD-F0EAD2D65308}" name="IN: Radius (cm)"/>
+    <tableColumn id="2" xr3:uid="{9B98FDBD-C297-4487-AF68-5D76CCFC8A84}" name="IN: Height (cm)"/>
+    <tableColumn id="3" xr3:uid="{A9EF7966-6285-4C21-9943-7E0C14D31EEC}" name="OUT: Volume (ML)">
+      <calculatedColumnFormula>(A2 ^ 2) * B2 * 3.14159265358979</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{FC1B8999-9CDB-4F3C-B75A-7CFD7939C0EC}" name="OUT: Cups">
+      <calculatedColumnFormula>C2 / 236</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -440,15 +488,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47C2D28A-397B-413C-A21F-3B6D2FD92EBE}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="10" width="20.77734375" customWidth="1"/>
+    <col min="1" max="4" width="20.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -456,13 +504,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -497,9 +545,64 @@
         <v>0.99838749584421294</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <f>(A4 ^ 2) * B4 * 3.14159265358979</f>
+        <v>452.38934211692975</v>
+      </c>
+      <c r="D4">
+        <f>C4 / 236</f>
+        <v>1.9169039920208888</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:C6" si="0">(A5 ^ 2) * B5 * 3.14159265358979</f>
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:D6" si="1">C5 / 236</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>785.39816339744755</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>3.3279583194807101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Tests and outputs verified -Cooper
</commit_message>
<xml_diff>
--- a/testcases.xlsx
+++ b/testcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nmare\PycharmProjects\cs151-pa0-CooperNaz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C13D31-4BB0-49DF-9B68-F692A020D995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6063FA-AFFF-4C3F-AEC4-7FF31ED86784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{3FADB8AC-B405-4FE2-9A10-87DD62C18585}"/>
+    <workbookView xWindow="2352" yWindow="3672" windowWidth="17280" windowHeight="10008" xr2:uid="{3FADB8AC-B405-4FE2-9A10-87DD62C18585}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>IN: Radius (cm)</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>OUT: Cups</t>
-  </si>
-  <si>
-    <t>The actual code rounds to the second decimal point. This does not account for that.</t>
   </si>
 </sst>
 </file>
@@ -488,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47C2D28A-397B-413C-A21F-3B6D2FD92EBE}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -569,11 +566,11 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <f t="shared" ref="C5:C6" si="0">(A5 ^ 2) * B5 * 3.14159265358979</f>
+        <f>(A5 ^ 2) * B5 * 3.14159265358979</f>
         <v>0</v>
       </c>
       <c r="D5">
-        <f t="shared" ref="D5:D6" si="1">C5 / 236</f>
+        <f t="shared" ref="D5:D6" si="0">C5 / 236</f>
         <v>0</v>
       </c>
     </row>
@@ -585,17 +582,12 @@
         <v>10</v>
       </c>
       <c r="C6">
+        <f>(A6 ^ 2) * B6 * 3.14159265358979</f>
+        <v>785.39816339744755</v>
+      </c>
+      <c r="D6">
         <f t="shared" si="0"/>
-        <v>785.39816339744755</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="1"/>
         <v>3.3279583194807101</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -607,6 +599,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001BA90F038B774F4697EE27A231644A3D" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1394086af1d3007eb5ee1d0ef65b36d2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0ff1ab6f-70c6-4f6a-a6d3-b571283720f7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="21cc815cb5b538b30358ec00d9d1dd23" ns3:_="">
     <xsd:import namespace="0ff1ab6f-70c6-4f6a-a6d3-b571283720f7"/>
@@ -762,15 +763,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -780,6 +772,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C827B6F-29A3-4BF0-961E-AE0557703ED0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D295DB4-02D8-4469-BC59-C2A2388DDF04}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -797,14 +797,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C827B6F-29A3-4BF0-961E-AE0557703ED0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B15DEC00-9A3F-48D7-B009-2E7D2FD8787A}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Messed with Excel a bit -Cooper
</commit_message>
<xml_diff>
--- a/testcases.xlsx
+++ b/testcases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nmare\PycharmProjects\cs151-pa0-CooperNaz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6063FA-AFFF-4C3F-AEC4-7FF31ED86784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A2A913-F3E4-42DB-8BE8-16736A0CFA1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2352" yWindow="3672" windowWidth="17280" windowHeight="10008" xr2:uid="{3FADB8AC-B405-4FE2-9A10-87DD62C18585}"/>
   </bookViews>
@@ -599,15 +599,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001BA90F038B774F4697EE27A231644A3D" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1394086af1d3007eb5ee1d0ef65b36d2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0ff1ab6f-70c6-4f6a-a6d3-b571283720f7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="21cc815cb5b538b30358ec00d9d1dd23" ns3:_="">
     <xsd:import namespace="0ff1ab6f-70c6-4f6a-a6d3-b571283720f7"/>
@@ -763,6 +754,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -772,14 +772,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C827B6F-29A3-4BF0-961E-AE0557703ED0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D295DB4-02D8-4469-BC59-C2A2388DDF04}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -797,6 +789,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C827B6F-29A3-4BF0-961E-AE0557703ED0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B15DEC00-9A3F-48D7-B009-2E7D2FD8787A}">
   <ds:schemaRefs>

</xml_diff>